<commit_message>
Changes to be committed: modified:   RTS CAP/Simulated Data/Book.xlsx modified:   RTS CAP/TaskLoader.py
Excel can now properly load the data from the Book.xlsx file.
</commit_message>
<xml_diff>
--- a/RTS CAP/Simulated Data/Book.xlsx
+++ b/RTS CAP/Simulated Data/Book.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A90BAA6-AB44-4588-A496-BB074EF98C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e157f4cbda4ef536/Desktop/Capstone CS698/Code/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{8D3B39A3-D1B9-42D6-B27F-6C4BE20E0653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82FB564B-B57E-496E-BDD0-024FF3AD9D1C}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29475" yWindow="2370" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,24 +38,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
-    <t>TaskID</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
     <t>Period</t>
   </si>
   <si>
-    <t>ExecutionTime</t>
-  </si>
-  <si>
     <t>Deadline</t>
   </si>
   <si>
-    <t>ResourceReq</t>
-  </si>
-  <si>
     <t>T1</t>
   </si>
   <si>
@@ -61,13 +57,22 @@
   </si>
   <si>
     <t>T3</t>
+  </si>
+  <si>
+    <t>Task ID</t>
+  </si>
+  <si>
+    <t>Execution Time</t>
+  </si>
+  <si>
+    <t>Resource Requirements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,10 +450,10 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
@@ -458,29 +463,29 @@
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>6</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -495,12 +500,12 @@
         <v>50</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -515,12 +520,12 @@
         <v>100</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -535,7 +540,7 @@
         <v>200</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>